<commit_message>
Electronic -> BOM update: C,L from Buck-Conv.
</commit_message>
<xml_diff>
--- a/Electronic/Production/BOM_ZumoComSystem.xlsx
+++ b/Electronic/Production/BOM_ZumoComSystem.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>ZumoComSystem</t>
   </si>
@@ -74,9 +74,6 @@
     <t>USB-A Buchse</t>
   </si>
   <si>
-    <t>USB-C Buchse</t>
-  </si>
-  <si>
     <t>ESP32 Modul</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t xml:space="preserve">534-1043 </t>
   </si>
   <si>
-    <t>WE 632723300011</t>
-  </si>
-  <si>
     <t>TL3301FF160QG</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>Schutzschaltung Batterie</t>
   </si>
   <si>
-    <t>1965-ESP32-WROOM-32E(4MBHIGHTEMP)CT-ND</t>
-  </si>
-  <si>
     <t>ESP32</t>
   </si>
   <si>
@@ -159,16 +150,36 @@
   </si>
   <si>
     <t>MOSFET P-Kanal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/central-semiconductor-corp/CXDM4060P-TR-PBFREE/1514-CXDM4060PTRPBFREECT-ND/4807155</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 40V 6A SOT-89</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/espressif-systems/ESP32-WROOM-32D-16MB/1904-1025-1-ND/9381734</t>
+  </si>
+  <si>
+    <t>Micro-USB Buchse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,14 +202,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,7 +494,7 @@
   <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,21 +536,21 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -563,18 +577,15 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -585,27 +596,27 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>34</v>
+      <c r="F11" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -632,7 +643,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -643,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -651,66 +662,84 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>25</v>
+      <c r="F17" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
-        <v>40</v>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
-        <v>42</v>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>38</v>
+      <c r="F20" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F18" r:id="rId1"/>
+    <hyperlink ref="F19" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
+    <hyperlink ref="F20" r:id="rId5"/>
+    <hyperlink ref="F21" r:id="rId6"/>
+    <hyperlink ref="F17" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
electronic: BOM: n-mosfet; SMD-pin correct position
</commit_message>
<xml_diff>
--- a/Electronic/Production/BOM_ZumoComSystem.xlsx
+++ b/Electronic/Production/BOM_ZumoComSystem.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
   <si>
     <t>ZumoComSystem</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>LED YELLOW DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>MOSFET n-Kanal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/toshiba-semiconductor-and-storage/SSM3K72CFS-LF/SSM3K72CFSLFCT-ND/5977741</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>SSM3K72CFS,LF</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1075,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A4:L36" totalsRowShown="0" tableBorderDxfId="12">
-  <autoFilter ref="A4:L36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A4:L37" totalsRowShown="0" tableBorderDxfId="12">
+  <autoFilter ref="A4:L37"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Bezeichnung" dataDxfId="11"/>
     <tableColumn id="10" name="Kürzel" dataDxfId="10"/>
@@ -1346,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L36"/>
+  <dimension ref="A2:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,23 +1962,21 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F28" s="8">
-        <v>3</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="7" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1974,23 +1984,23 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F29" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1998,15 +2008,15 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F30" s="8">
         <v>1</v>
@@ -2014,7 +2024,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2022,7 +2032,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2030,7 +2040,7 @@
         <v>48</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F31" s="8">
         <v>1</v>
@@ -2038,7 +2048,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="7" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2046,7 +2056,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2054,7 +2064,7 @@
         <v>48</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F32" s="8">
         <v>1</v>
@@ -2062,7 +2072,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -2070,7 +2080,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2078,7 +2088,7 @@
         <v>48</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F33" s="8">
         <v>1</v>
@@ -2086,7 +2096,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2094,71 +2104,95 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E34" s="6" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="F34" s="8">
         <v>1</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="I34" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="12"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="F35" s="8">
         <v>1</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="8">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="12"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E37" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="16">
-        <v>1</v>
-      </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="17" t="s">
+      <c r="F37" s="16">
+        <v>1</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="1"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2168,9 +2202,9 @@
     <hyperlink ref="I15" r:id="rId4"/>
     <hyperlink ref="I18" r:id="rId5"/>
     <hyperlink ref="I19" r:id="rId6"/>
-    <hyperlink ref="I36" r:id="rId7"/>
+    <hyperlink ref="I37" r:id="rId7"/>
     <hyperlink ref="I11" r:id="rId8"/>
-    <hyperlink ref="I35" r:id="rId9"/>
+    <hyperlink ref="I36" r:id="rId9"/>
     <hyperlink ref="I7" r:id="rId10"/>
     <hyperlink ref="I6" r:id="rId11"/>
     <hyperlink ref="I8" r:id="rId12"/>
@@ -2179,10 +2213,10 @@
     <hyperlink ref="I21" r:id="rId15"/>
     <hyperlink ref="I22" r:id="rId16"/>
     <hyperlink ref="I25" r:id="rId17"/>
-    <hyperlink ref="I30" r:id="rId18"/>
-    <hyperlink ref="I31" r:id="rId19"/>
-    <hyperlink ref="I33" r:id="rId20"/>
-    <hyperlink ref="I29" r:id="rId21"/>
+    <hyperlink ref="I31" r:id="rId18"/>
+    <hyperlink ref="I32" r:id="rId19"/>
+    <hyperlink ref="I34" r:id="rId20"/>
+    <hyperlink ref="I30" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>

</xml_diff>